<commit_message>
Suggestions for better layout
</commit_message>
<xml_diff>
--- a/handkontroll/layout.xlsx
+++ b/handkontroll/layout.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\GitHub\Arduino_material\handkontroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0EB20F-74A3-40CC-A143-54B5493E7D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633097FA-7F8E-486B-9B91-735398651BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15810" windowHeight="9945" xr2:uid="{10B6FF37-F49A-414B-BF0C-8080337D09B8}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15810" windowHeight="9945" activeTab="1" xr2:uid="{10B6FF37-F49A-414B-BF0C-8080337D09B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Suggestions" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>%</t>
   </si>
@@ -91,6 +92,42 @@
   </si>
   <si>
     <t>:</t>
+  </si>
+  <si>
+    <t>RUN MOTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP MOTOR </t>
+  </si>
+  <si>
+    <t>MOTOR STOPPED  &lt;%  &lt;s</t>
+  </si>
+  <si>
+    <t>FORWARD AT ###%</t>
+  </si>
+  <si>
+    <t>REVERSE AT ###%</t>
+  </si>
+  <si>
+    <t>For ##s</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
+  </si>
+  <si>
+    <t>##s remaining at</t>
+  </si>
+  <si>
+    <t>###% forward speed</t>
+  </si>
+  <si>
+    <t>###% reverse speed</t>
+  </si>
+  <si>
+    <t>0s No time set</t>
+  </si>
+  <si>
+    <t>TRY THESE!</t>
   </si>
 </sst>
 </file>
@@ -147,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,6 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365D3F38-3556-4FE5-83C4-B82F310AE819}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +713,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A7B044-F1CF-46A1-8791-9FD55C3C8E09}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="str">
+        <f>"  0% Increase speed"</f>
+        <v xml:space="preserve">  0% Increase speed</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="str">
+        <f>"  0% No speed set"</f>
+        <v xml:space="preserve">  0% No speed set</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48598591-4342-47EF-9DEB-3A356C5646FE}">
   <dimension ref="A2:B4"/>
   <sheetViews>

</xml_diff>